<commit_message>
Commit automatique via PowerShell
</commit_message>
<xml_diff>
--- a/liste groupe 1.xlsx
+++ b/liste groupe 1.xlsx
@@ -247,8 +247,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="5">
     <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
@@ -306,28 +311,61 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="19">
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" xfId="0" applyProtection="1"/>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" xfId="0" applyProtection="1" applyAlignment="1">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="4" applyFont="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" xfId="0" applyProtection="1" applyAlignment="1">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="2" applyFill="1" borderId="1" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="2" applyFill="1" borderId="1" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" borderId="2" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" borderId="2" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" borderId="2" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" borderId="2" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" borderId="2" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" xfId="0" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="2" applyFill="1" borderId="1" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" borderId="2" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" borderId="2" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" borderId="2" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" borderId="2" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" borderId="2" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -345,12 +383,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="19.2416572570801" customWidth="1"/>
-    <col min="3" max="3" width="15.082896232605" customWidth="1"/>
-    <col min="4" max="4" width="19.4687786102295" customWidth="1"/>
+    <col min="1" max="1" width="3.29" customWidth="1" style="6"/>
+    <col min="2" max="2" width="20.14" customWidth="1" style="9"/>
+    <col min="3" max="3" width="15.43" customWidth="1" style="9"/>
+    <col min="4" max="4" width="11.8" customWidth="1" style="16"/>
     <col min="5" max="5" width="12.1313533782959" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" customWidth="1"/>
-    <col min="7" max="7" width="19.7143135070801" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" customWidth="1" style="16"/>
+    <col min="7" max="7" width="15.1" customWidth="1" style="16"/>
     <col min="8" max="8" width="12.3809814453125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -358,464 +397,534 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
     </row>
     <row r="3" ht="30" customHeight="1">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4" t="s">
+      <c r="A3" s="3"/>
+      <c r="B3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" ht="30" customHeight="1">
-      <c r="A4" s="5">
+    <row r="4" ht="40" customHeight="1">
+      <c r="A4" s="7">
         <v>1</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" ht="30" customHeight="1">
-      <c r="A5" s="5">
+      <c r="H4" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" ht="40" customHeight="1">
+      <c r="A5" s="7">
         <v>2</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" ht="30" customHeight="1">
-      <c r="A6" s="5">
+      <c r="H5" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" ht="40" customHeight="1">
+      <c r="A6" s="7">
         <v>3</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G6" s="5" t="s">
+      <c r="F6" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" ht="30" customHeight="1">
-      <c r="A7" s="5">
+      <c r="H6" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" ht="40" customHeight="1">
+      <c r="A7" s="7">
         <v>4</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="H7" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" ht="30" customHeight="1">
-      <c r="A8" s="5">
+      <c r="H7" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" ht="40" customHeight="1">
+      <c r="A8" s="7">
         <v>5</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G8" s="5" t="s">
+      <c r="F8" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="H8" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" ht="30" customHeight="1">
-      <c r="A9" s="5">
+      <c r="H8" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" ht="40" customHeight="1">
+      <c r="A9" s="7">
         <v>6</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G9" s="5" t="s">
+      <c r="F9" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="H9" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" ht="30" customHeight="1">
-      <c r="A10" s="5">
+      <c r="H9" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" ht="40" customHeight="1">
+      <c r="A10" s="7">
         <v>7</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="F10" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G10" s="5" t="s">
+      <c r="F10" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="H10" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" ht="30" customHeight="1">
-      <c r="A11" s="5">
+      <c r="H10" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" ht="40" customHeight="1">
+      <c r="A11" s="7">
         <v>8</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="G11" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="H11" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" ht="30" customHeight="1">
-      <c r="A12" s="5">
+      <c r="H11" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" ht="40" customHeight="1">
+      <c r="A12" s="7">
         <v>9</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F12" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G12" s="5" t="s">
+      <c r="F12" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="H12" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" ht="30" customHeight="1">
-      <c r="A13" s="5">
+      <c r="H12" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" ht="40" customHeight="1">
+      <c r="A13" s="7">
         <v>10</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="F13" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G13" s="5" t="s">
+      <c r="F13" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="G13" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="H13" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" ht="30" customHeight="1">
-      <c r="A14" s="5">
+      <c r="H13" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" ht="40" customHeight="1">
+      <c r="A14" s="7">
         <v>11</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="F14" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G14" s="5" t="s">
+      <c r="F14" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="G14" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="H14" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" ht="30" customHeight="1">
-      <c r="A15" s="5">
+      <c r="H14" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" ht="40" customHeight="1">
+      <c r="A15" s="7">
         <v>12</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="F15" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G15" s="5" t="s">
+      <c r="F15" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="G15" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="H15" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" ht="30" customHeight="1">
-      <c r="A16" s="5">
+      <c r="H15" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" ht="40" customHeight="1">
+      <c r="A16" s="7">
         <v>13</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E16" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="F16" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G16" s="5" t="s">
+      <c r="F16" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="G16" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="H16" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" ht="30" customHeight="1">
-      <c r="A17" s="5">
+      <c r="H16" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" ht="40" customHeight="1">
+      <c r="A17" s="7">
         <v>14</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E17" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F17" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G17" s="5" t="s">
+      <c r="F17" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="G17" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="H17" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" ht="30" customHeight="1">
-      <c r="A18" s="5">
-        <v>15</v>
-      </c>
-      <c r="B18" s="6" t="s">
+      <c r="H17" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" ht="40" customHeight="1">
+      <c r="A18" s="7">
+        <v>15</v>
+      </c>
+      <c r="B18" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E18" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="F18" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G18" s="5" t="s">
+      <c r="F18" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="G18" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="H18" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" ht="30" customHeight="1">
-      <c r="A19" s="7">
+      <c r="H18" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" ht="40" customHeight="1">
+      <c r="A19" s="8">
         <v>16</v>
       </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-    </row>
-    <row r="20" ht="30" customHeight="1">
-      <c r="A20" s="7">
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="5"/>
+    </row>
+    <row r="20" ht="40" customHeight="1">
+      <c r="A20" s="8">
         <v>17</v>
       </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-    </row>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="5"/>
+    </row>
+    <row r="21" ht="40" customHeight="1"/>
+    <row r="22" ht="40" customHeight="1"/>
+    <row r="23" ht="40" customHeight="1"/>
+    <row r="24" ht="40" customHeight="1"/>
+    <row r="25" ht="40" customHeight="1"/>
+    <row r="26" ht="40" customHeight="1"/>
+    <row r="27" ht="40" customHeight="1"/>
+    <row r="28" ht="40" customHeight="1"/>
+    <row r="29" ht="40" customHeight="1"/>
+    <row r="30" ht="40" customHeight="1"/>
+    <row r="31" ht="40" customHeight="1"/>
+    <row r="32" ht="40" customHeight="1"/>
+    <row r="33" ht="40" customHeight="1"/>
+    <row r="34" ht="40" customHeight="1"/>
+    <row r="35" ht="40" customHeight="1"/>
+    <row r="36" ht="40" customHeight="1"/>
+    <row r="37" ht="40" customHeight="1"/>
+    <row r="38" ht="40" customHeight="1"/>
+    <row r="39" ht="40" customHeight="1"/>
+    <row r="40" ht="40" customHeight="1"/>
+    <row r="41" ht="40" customHeight="1"/>
+    <row r="42" ht="40" customHeight="1"/>
+    <row r="43" ht="40" customHeight="1"/>
+    <row r="44" ht="40" customHeight="1"/>
+    <row r="45" ht="40" customHeight="1"/>
+    <row r="46" ht="40" customHeight="1"/>
+    <row r="47" ht="40" customHeight="1"/>
+    <row r="48" ht="40" customHeight="1"/>
+    <row r="49" ht="40" customHeight="1"/>
+    <row r="50" ht="40" customHeight="1"/>
+    <row r="51" ht="40" customHeight="1"/>
+    <row r="52" ht="40" customHeight="1"/>
+    <row r="53" ht="40" customHeight="1"/>
+    <row r="54" ht="40" customHeight="1"/>
+    <row r="55" ht="40" customHeight="1"/>
+    <row r="56" ht="40" customHeight="1"/>
+    <row r="57" ht="40" customHeight="1"/>
+    <row r="58" ht="40" customHeight="1"/>
+    <row r="59" ht="40" customHeight="1"/>
+    <row r="60" ht="40" customHeight="1"/>
+    <row r="61" ht="40" customHeight="1"/>
+    <row r="62" ht="40" customHeight="1"/>
+    <row r="63" ht="40" customHeight="1"/>
+    <row r="64" ht="40" customHeight="1"/>
+    <row r="65" ht="40" customHeight="1"/>
+    <row r="66" ht="40" customHeight="1"/>
+    <row r="67" ht="40" customHeight="1"/>
+    <row r="68" ht="40" customHeight="1"/>
+    <row r="69" ht="40" customHeight="1"/>
+    <row r="70" ht="40" customHeight="1"/>
+    <row r="71" ht="40" customHeight="1"/>
+    <row r="72" ht="40" customHeight="1"/>
+    <row r="73" ht="40" customHeight="1"/>
+    <row r="74" ht="40" customHeight="1"/>
+    <row r="75" ht="40" customHeight="1"/>
+    <row r="76" ht="40" customHeight="1"/>
+    <row r="77" ht="40" customHeight="1"/>
+    <row r="78" ht="40" customHeight="1"/>
+    <row r="79" ht="40" customHeight="1"/>
+    <row r="80" ht="40" customHeight="1"/>
+    <row r="81" ht="40" customHeight="1"/>
+    <row r="82" ht="40" customHeight="1"/>
+    <row r="83" ht="40" customHeight="1"/>
+    <row r="84" ht="40" customHeight="1"/>
+    <row r="85" ht="40" customHeight="1"/>
+    <row r="86" ht="40" customHeight="1"/>
+    <row r="87" ht="40" customHeight="1"/>
+    <row r="88" ht="40" customHeight="1"/>
+    <row r="89" ht="40" customHeight="1"/>
+    <row r="90" ht="40" customHeight="1"/>
   </sheetData>
   <mergeCells>
     <mergeCell ref="A1:H1"/>

</xml_diff>